<commit_message>
N1 N2 met BNR requirements
</commit_message>
<xml_diff>
--- a/exposan/werf/data/ic.xlsx
+++ b/exposan/werf/data/ic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joy_c\Dropbox\PhD\Research\QSD\codes_developing\EXPOsan\exposan\werf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EBC8A1A-7505-4AE8-9A4E-E8BD9A708E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B90C454-39E1-46E2-BA9D-4D59A065EA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="1800" windowWidth="18795" windowHeight="16050" firstSheet="6" activeTab="14" xr2:uid="{218DD762-44D5-4240-B5CB-C558EBE30BA7}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="19455" windowHeight="16050" firstSheet="6" activeTab="17" xr2:uid="{218DD762-44D5-4240-B5CB-C558EBE30BA7}"/>
   </bookViews>
   <sheets>
     <sheet name="B1" sheetId="6" r:id="rId1"/>
@@ -5174,7 +5174,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42016BA4-57DB-462D-9767-837B2F986A82}">
   <dimension ref="A1:AE16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
@@ -5912,7 +5912,7 @@
   <dimension ref="A1:AE16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6013,29 +6013,29 @@
       <c r="A2" t="s">
         <v>59</v>
       </c>
-      <c r="B2">
-        <v>1E-3</v>
+      <c r="B2" s="1">
+        <v>1E-4</v>
       </c>
       <c r="C2">
         <v>18</v>
       </c>
       <c r="D2">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E2">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="F2">
         <v>22</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H2">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="I2">
-        <v>17.8999643029649</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="J2">
         <v>65</v>
@@ -6047,43 +6047,43 @@
         <v>50</v>
       </c>
       <c r="M2">
-        <v>30000</v>
+        <v>2000</v>
       </c>
       <c r="N2">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="O2">
-        <v>700</v>
+        <v>1000</v>
       </c>
       <c r="P2">
         <v>500</v>
       </c>
       <c r="Q2">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="R2">
         <v>40</v>
       </c>
       <c r="S2">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="T2">
         <v>140</v>
       </c>
-      <c r="U2">
-        <v>0.01</v>
+      <c r="U2" s="1">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="V2">
         <v>0.3</v>
       </c>
-      <c r="W2">
-        <v>0.3</v>
+      <c r="W2" s="1">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="X2">
         <v>0.1</v>
       </c>
-      <c r="Y2">
-        <v>0.05</v>
+      <c r="Y2" s="1">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="Z2" s="1">
         <v>9.9999999999999995E-7</v>
@@ -6115,22 +6115,22 @@
         <v>18</v>
       </c>
       <c r="D3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3">
-        <v>3</v>
+        <v>0.3</v>
       </c>
       <c r="F3">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="I3">
-        <v>17.8999643029649</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="J3">
         <v>40</v>
@@ -6142,43 +6142,43 @@
         <v>50</v>
       </c>
       <c r="M3">
-        <v>30000</v>
+        <v>2000</v>
       </c>
       <c r="N3">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="O3">
-        <v>1300</v>
+        <v>2000</v>
       </c>
       <c r="P3">
         <v>1000</v>
       </c>
       <c r="Q3">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="R3">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="S3">
-        <v>220</v>
+        <v>120</v>
       </c>
       <c r="T3">
         <v>140</v>
       </c>
-      <c r="U3">
-        <v>0.01</v>
+      <c r="U3" s="1">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="V3">
         <v>0.1</v>
       </c>
-      <c r="W3">
-        <v>0.2</v>
+      <c r="W3" s="1">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="X3">
         <v>0.05</v>
       </c>
-      <c r="Y3">
-        <v>0.02</v>
+      <c r="Y3" s="1">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="Z3" s="1">
         <v>9.9999999999999995E-7</v>
@@ -6204,28 +6204,28 @@
         <v>68</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>18</v>
       </c>
       <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4">
         <v>1</v>
       </c>
-      <c r="E4">
-        <v>7</v>
-      </c>
-      <c r="F4">
-        <v>6</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
       <c r="H4">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="I4">
-        <v>17.8999643029649</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="J4">
         <v>25</v>
@@ -6237,43 +6237,43 @@
         <v>50</v>
       </c>
       <c r="M4">
-        <v>30000</v>
+        <v>2000</v>
       </c>
       <c r="N4">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="O4">
-        <v>1700</v>
+        <v>2000</v>
       </c>
       <c r="P4">
-        <v>1200</v>
+        <v>1000</v>
       </c>
       <c r="Q4">
-        <v>400</v>
+        <v>350</v>
       </c>
       <c r="R4">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="S4">
-        <v>270</v>
+        <v>150</v>
       </c>
       <c r="T4">
         <v>140</v>
       </c>
-      <c r="U4">
-        <v>0.01</v>
+      <c r="U4" s="1">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="V4">
         <v>0.01</v>
       </c>
-      <c r="W4">
-        <v>0.1</v>
+      <c r="W4" s="1">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="X4">
         <v>0.05</v>
       </c>
-      <c r="Y4">
-        <v>0.02</v>
+      <c r="Y4" s="1">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="Z4" s="1">
         <v>9.9999999999999995E-7</v>
@@ -6299,7 +6299,7 @@
         <v>69</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>18</v>
@@ -6308,19 +6308,19 @@
         <v>0.5</v>
       </c>
       <c r="E5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="I5">
-        <v>17.8999643029649</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="J5">
         <v>20</v>
@@ -6332,43 +6332,43 @@
         <v>50</v>
       </c>
       <c r="M5">
-        <v>30000</v>
+        <v>2000</v>
       </c>
       <c r="N5">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="O5">
-        <v>1700</v>
+        <v>2000</v>
       </c>
       <c r="P5">
-        <v>1200</v>
+        <v>1000</v>
       </c>
       <c r="Q5">
-        <v>400</v>
+        <v>350</v>
       </c>
       <c r="R5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="S5">
-        <v>270</v>
+        <v>150</v>
       </c>
       <c r="T5">
         <v>140</v>
       </c>
-      <c r="U5">
-        <v>0.01</v>
+      <c r="U5" s="1">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="V5">
         <v>0.01</v>
       </c>
-      <c r="W5">
-        <v>0.1</v>
+      <c r="W5" s="1">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="X5">
         <v>0.01</v>
       </c>
-      <c r="Y5">
-        <v>0.02</v>
+      <c r="Y5" s="1">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="Z5" s="1">
         <v>9.9999999999999995E-7</v>
@@ -6403,19 +6403,19 @@
         <v>0.5</v>
       </c>
       <c r="E6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>20</v>
+        <v>0.1</v>
       </c>
       <c r="I6">
-        <v>17.8999643029649</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="J6">
         <v>20</v>
@@ -6427,43 +6427,43 @@
         <v>50</v>
       </c>
       <c r="M6">
-        <v>30000</v>
+        <v>2000</v>
       </c>
       <c r="N6">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="O6">
-        <v>1700</v>
+        <v>2000</v>
       </c>
       <c r="P6">
-        <v>1200</v>
+        <v>1000</v>
       </c>
       <c r="Q6">
-        <v>400</v>
+        <v>350</v>
       </c>
       <c r="R6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S6">
-        <v>270</v>
+        <v>150</v>
       </c>
       <c r="T6">
         <v>140</v>
       </c>
-      <c r="U6">
-        <v>0.01</v>
+      <c r="U6" s="1">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="V6">
         <v>0.01</v>
       </c>
-      <c r="W6">
-        <v>0.1</v>
+      <c r="W6" s="1">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="X6">
         <v>0.01</v>
       </c>
-      <c r="Y6">
-        <v>0.02</v>
+      <c r="Y6" s="1">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="Z6" s="1">
         <v>9.9999999999999995E-7</v>
@@ -6495,25 +6495,25 @@
         <v>18</v>
       </c>
       <c r="D7">
+        <v>0.2</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
         <v>0.1</v>
       </c>
-      <c r="E7">
-        <v>7</v>
-      </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-      <c r="G7">
-        <v>2</v>
-      </c>
-      <c r="H7">
-        <v>18</v>
-      </c>
       <c r="I7">
-        <v>17.8999643029649</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="J7">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K7">
         <v>28</v>
@@ -6522,43 +6522,43 @@
         <v>50</v>
       </c>
       <c r="M7">
-        <v>30000</v>
+        <v>2000</v>
       </c>
       <c r="N7">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="O7">
-        <v>2100</v>
+        <v>3000</v>
       </c>
       <c r="P7">
         <v>1500</v>
       </c>
       <c r="Q7">
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="R7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S7">
-        <v>340</v>
+        <v>200</v>
       </c>
       <c r="T7">
         <v>140</v>
       </c>
-      <c r="U7">
-        <v>0.01</v>
+      <c r="U7" s="1">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="V7">
         <v>0.01</v>
       </c>
-      <c r="W7">
-        <v>0.1</v>
+      <c r="W7" s="1">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="X7">
         <v>0.01</v>
       </c>
-      <c r="Y7">
-        <v>0.02</v>
+      <c r="Y7" s="1">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="Z7" s="1">
         <v>9.9999999999999995E-7</v>
@@ -6633,18 +6633,6 @@
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
       <c r="AC14" s="1"/>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="R15" s="1"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
-      <c r="W15" s="1"/>
-      <c r="X15" s="1"/>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
-      <c r="AA15" s="1"/>
-      <c r="AB15" s="1"/>
-      <c r="AC15" s="1"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="R16" s="1"/>
@@ -7362,8 +7350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{472A4E84-05F6-482F-94AF-2C8CE149BF8E}">
   <dimension ref="A1:AP59"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8407,109 +8395,109 @@
         <v>72</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C9">
-        <v>0.5</v>
+        <v>6</v>
       </c>
       <c r="D9">
-        <v>7</v>
+        <v>120</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="H9">
-        <v>7</v>
+        <v>70</v>
       </c>
       <c r="I9">
-        <v>1E-4</v>
+        <v>2.8600000000000001E-4</v>
       </c>
       <c r="J9">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="K9">
-        <v>750</v>
+        <v>900</v>
       </c>
       <c r="L9">
-        <v>1500</v>
+        <v>1200</v>
       </c>
       <c r="M9">
-        <v>250</v>
+        <v>1200</v>
       </c>
       <c r="N9">
         <v>17.899999999999999</v>
       </c>
       <c r="O9">
-        <v>10</v>
+        <v>1800</v>
       </c>
       <c r="P9">
-        <v>10</v>
+        <v>1800</v>
       </c>
       <c r="Q9">
-        <v>10</v>
+        <v>2500</v>
       </c>
       <c r="R9">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="S9">
-        <v>1000</v>
+        <v>550</v>
       </c>
       <c r="T9">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="U9">
-        <v>650</v>
+        <v>220</v>
       </c>
       <c r="V9">
+        <v>120</v>
+      </c>
+      <c r="W9">
+        <v>700</v>
+      </c>
+      <c r="X9">
         <v>350</v>
       </c>
-      <c r="W9">
-        <v>850</v>
-      </c>
-      <c r="X9">
+      <c r="Y9">
+        <v>20000</v>
+      </c>
+      <c r="Z9">
+        <v>865</v>
+      </c>
+      <c r="AA9">
+        <v>1</v>
+      </c>
+      <c r="AB9">
+        <v>1200</v>
+      </c>
+      <c r="AC9">
         <v>600</v>
       </c>
-      <c r="Y9">
-        <v>32000</v>
-      </c>
-      <c r="Z9">
-        <v>65</v>
-      </c>
-      <c r="AA9">
-        <v>0.01</v>
-      </c>
-      <c r="AB9">
-        <v>80</v>
-      </c>
-      <c r="AC9">
-        <v>60</v>
-      </c>
       <c r="AD9">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="AE9">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="AF9" s="1">
-        <v>0.1</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="AG9">
-        <v>950</v>
-      </c>
-      <c r="AH9">
-        <v>0.02</v>
+        <v>4000</v>
+      </c>
+      <c r="AH9" s="1">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="AI9">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="AJ9" s="1">
-        <v>0.01</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="AK9" s="1">
         <v>1.0000000000000001E-5</v>
@@ -8659,16 +8647,16 @@
       </c>
     </row>
     <row r="11" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="K11" s="1"/>
-      <c r="AA11" s="1"/>
-      <c r="AF11" s="1"/>
-      <c r="AH11" s="1"/>
-      <c r="AJ11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AE11" s="1"/>
+      <c r="AG11" s="1"/>
+      <c r="AI11" s="1"/>
+      <c r="AK11" s="1"/>
       <c r="AL11" s="1"/>
       <c r="AM11" s="1"/>
       <c r="AN11" s="1"/>
       <c r="AO11" s="1"/>
-      <c r="AP11" s="1"/>
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="D13" s="1"/>

</xml_diff>

<commit_message>
G2 met BNR requirements
</commit_message>
<xml_diff>
--- a/exposan/werf/data/ic.xlsx
+++ b/exposan/werf/data/ic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joy_c\Dropbox\PhD\Research\QSD\codes_developing\EXPOsan\exposan\werf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B90C454-39E1-46E2-BA9D-4D59A065EA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C83BE2-93A1-4BBC-A23E-21E33BD3A455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="19455" windowHeight="16050" firstSheet="6" activeTab="17" xr2:uid="{218DD762-44D5-4240-B5CB-C558EBE30BA7}"/>
+    <workbookView xWindow="-23133" yWindow="-93" windowWidth="23226" windowHeight="13866" firstSheet="6" activeTab="16" xr2:uid="{218DD762-44D5-4240-B5CB-C558EBE30BA7}"/>
   </bookViews>
   <sheets>
     <sheet name="B1" sheetId="6" r:id="rId1"/>
@@ -6652,7 +6652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CB7F0C9-B54B-4F93-93CE-9E10B0EA4FF3}">
   <dimension ref="A1:AF7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AB6" sqref="AB6"/>
     </sheetView>
   </sheetViews>
@@ -7350,7 +7350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{472A4E84-05F6-482F-94AF-2C8CE149BF8E}">
   <dimension ref="A1:AP59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -13096,8 +13096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC5318B9-9FE8-4735-97AC-C84ECA362166}">
   <dimension ref="A1:AE15"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:R7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13793,7 +13793,7 @@
   <dimension ref="A1:AE38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13895,31 +13895,31 @@
         <v>59</v>
       </c>
       <c r="B2">
+        <v>0.01</v>
+      </c>
+      <c r="C2">
+        <v>18</v>
+      </c>
+      <c r="D2">
+        <v>0.05</v>
+      </c>
+      <c r="E2">
         <v>0.1</v>
       </c>
-      <c r="C2">
-        <v>25</v>
-      </c>
-      <c r="D2">
-        <v>0.01</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
       <c r="F2">
-        <v>0.4</v>
+        <v>100</v>
       </c>
       <c r="G2">
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="H2">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="I2">
         <v>18</v>
       </c>
       <c r="J2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="K2">
         <v>28</v>
@@ -13928,13 +13928,13 @@
         <v>50</v>
       </c>
       <c r="M2">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="N2">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="O2">
-        <v>2300</v>
+        <v>2000</v>
       </c>
       <c r="P2">
         <v>2000</v>
@@ -13943,10 +13943,10 @@
         <v>600</v>
       </c>
       <c r="R2">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="S2">
-        <v>250</v>
+        <v>150</v>
       </c>
       <c r="T2">
         <v>140</v>
@@ -13993,28 +13993,28 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D3">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E3">
         <v>0.01</v>
       </c>
       <c r="F3">
-        <v>0.5</v>
+        <v>60</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I3">
         <v>18</v>
       </c>
       <c r="J3">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="K3">
         <v>28</v>
@@ -14023,13 +14023,13 @@
         <v>50</v>
       </c>
       <c r="M3">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="N3">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="O3">
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="P3">
         <v>700</v>
@@ -14038,10 +14038,10 @@
         <v>200</v>
       </c>
       <c r="R3">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="S3">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="T3">
         <v>140</v>
@@ -14088,7 +14088,7 @@
         <v>0.01</v>
       </c>
       <c r="C4">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D4">
         <v>6</v>
@@ -14097,19 +14097,19 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>0.3</v>
+        <v>20</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="I4">
         <v>18</v>
       </c>
       <c r="J4">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="K4">
         <v>28</v>
@@ -14118,25 +14118,25 @@
         <v>50</v>
       </c>
       <c r="M4">
-        <v>900</v>
+        <v>500</v>
       </c>
       <c r="N4">
         <v>30</v>
       </c>
       <c r="O4">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="P4">
         <v>600</v>
       </c>
       <c r="Q4">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="R4">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="S4">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="T4">
         <v>140</v>
@@ -14183,28 +14183,28 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E5">
         <v>0.1</v>
       </c>
       <c r="F5">
-        <v>0.3</v>
+        <v>15</v>
       </c>
       <c r="G5">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="I5">
         <v>18</v>
       </c>
       <c r="J5">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="K5">
         <v>28</v>
@@ -14213,25 +14213,25 @@
         <v>50</v>
       </c>
       <c r="M5">
-        <v>900</v>
+        <v>500</v>
       </c>
       <c r="N5">
         <v>27</v>
       </c>
       <c r="O5">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="P5">
         <v>600</v>
       </c>
       <c r="Q5">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="R5">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="S5">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="T5">
         <v>140</v>
@@ -14278,28 +14278,28 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6">
         <v>3</v>
       </c>
       <c r="F6">
-        <v>0.2</v>
+        <v>5</v>
       </c>
       <c r="G6">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="H6">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="I6">
         <v>18</v>
       </c>
       <c r="J6">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="K6">
         <v>28</v>
@@ -14308,25 +14308,25 @@
         <v>50</v>
       </c>
       <c r="M6">
-        <v>900</v>
+        <v>500</v>
       </c>
       <c r="N6">
         <v>25</v>
       </c>
       <c r="O6">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="P6">
         <v>600</v>
       </c>
       <c r="Q6">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="R6">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="S6">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="T6">
         <v>140</v>
@@ -14373,28 +14373,28 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7">
-        <v>0.2</v>
+        <v>2</v>
       </c>
       <c r="G7">
         <v>0.3</v>
       </c>
       <c r="H7">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="I7">
         <v>18</v>
       </c>
       <c r="J7">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="K7">
         <v>28</v>
@@ -14403,25 +14403,25 @@
         <v>50</v>
       </c>
       <c r="M7">
-        <v>900</v>
+        <v>500</v>
       </c>
       <c r="N7">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="O7">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="P7">
         <v>600</v>
       </c>
       <c r="Q7">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="R7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S7">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="T7">
         <v>140</v>
@@ -14461,6 +14461,10 @@
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
@@ -14537,52 +14541,162 @@
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:29" x14ac:dyDescent="0.25">
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:29" x14ac:dyDescent="0.25">
       <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1"/>
+    </row>
+    <row r="19" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
       <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="1"/>
+    </row>
+    <row r="20" spans="2:29" x14ac:dyDescent="0.25">
       <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1"/>
+    </row>
+    <row r="21" spans="2:29" x14ac:dyDescent="0.25">
       <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="1"/>
+    </row>
+    <row r="22" spans="2:29" x14ac:dyDescent="0.25">
       <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="1"/>
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="1"/>
+    </row>
+    <row r="23" spans="2:29" x14ac:dyDescent="0.25">
       <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
+      <c r="AA23" s="1"/>
+      <c r="AB23" s="1"/>
+      <c r="AC23" s="1"/>
+    </row>
+    <row r="24" spans="2:29" x14ac:dyDescent="0.25">
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:29" x14ac:dyDescent="0.25">
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:29" x14ac:dyDescent="0.25">
       <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="1"/>
+      <c r="AB26" s="1"/>
+      <c r="AC26" s="1"/>
+    </row>
+    <row r="27" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
       <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+      <c r="AA27" s="1"/>
+      <c r="AB27" s="1"/>
+      <c r="AC27" s="1"/>
+    </row>
+    <row r="28" spans="2:29" x14ac:dyDescent="0.25">
       <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
+      <c r="AA28" s="1"/>
+      <c r="AB28" s="1"/>
+      <c r="AC28" s="1"/>
+    </row>
+    <row r="29" spans="2:29" x14ac:dyDescent="0.25">
       <c r="G29" s="1"/>
-    </row>
-    <row r="30" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="1"/>
+      <c r="AA29" s="1"/>
+      <c r="AB29" s="1"/>
+      <c r="AC29" s="1"/>
+    </row>
+    <row r="30" spans="2:29" x14ac:dyDescent="0.25">
       <c r="G30" s="1"/>
-    </row>
-    <row r="31" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
+      <c r="Z30" s="1"/>
+      <c r="AA30" s="1"/>
+      <c r="AB30" s="1"/>
+      <c r="AC30" s="1"/>
+    </row>
+    <row r="31" spans="2:29" x14ac:dyDescent="0.25">
       <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
+      <c r="AA31" s="1"/>
+      <c r="AB31" s="1"/>
+      <c r="AC31" s="1"/>
+    </row>
+    <row r="32" spans="2:29" x14ac:dyDescent="0.25">
       <c r="G32" s="1"/>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.25">

</xml_diff>